<commit_message>
[Documentation] Updated product and sprint backlog for sprint 3.
This update keeps everything up to date.
</commit_message>
<xml_diff>
--- a/sprints/sprint 3/Sprint 3 Backlog.xlsx
+++ b/sprints/sprint 3/Sprint 3 Backlog.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csuser\source\repos\CapstoneProject\sprints\sprint 3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6B7EA2-FEBD-445A-BA3A-688B8F5139E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="12852" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -211,34 +220,40 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -248,50 +263,47 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -481,27 +493,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="82.86"/>
-    <col customWidth="1" min="2" max="2" width="25.43"/>
-    <col customWidth="1" min="3" max="3" width="13.43"/>
-    <col customWidth="1" min="4" max="4" width="44.43"/>
-    <col customWidth="1" min="5" max="5" width="30.57"/>
+    <col min="1" max="1" width="82.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -533,7 +550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -550,7 +567,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -567,7 +584,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -584,7 +601,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -599,7 +616,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -616,7 +633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -633,7 +650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -650,7 +667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -667,7 +684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
@@ -684,7 +701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
@@ -701,7 +718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
@@ -718,7 +735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -735,7 +752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
@@ -752,7 +769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
@@ -769,7 +786,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -784,7 +801,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -801,7 +818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
@@ -818,7 +835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
@@ -835,7 +852,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>44</v>
       </c>
@@ -852,7 +869,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -866,7 +883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>47</v>
       </c>
@@ -880,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>50</v>
       </c>
@@ -895,7 +912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>17</v>
       </c>
@@ -912,7 +929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>52</v>
       </c>
@@ -929,7 +946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>53</v>
       </c>
@@ -946,7 +963,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>55</v>
       </c>
@@ -963,7 +980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>40</v>
       </c>
@@ -980,7 +997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>42</v>
       </c>
@@ -997,7 +1014,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>57</v>
       </c>
@@ -1014,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>59</v>
       </c>
@@ -1031,7 +1048,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>60</v>
       </c>
@@ -1048,7 +1065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>62</v>
       </c>
@@ -1065,7 +1082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>33</v>
       </c>
@@ -1082,10 +1099,10 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>